<commit_message>
update Avalon and not reslove error
</commit_message>
<xml_diff>
--- a/Doc/需求分析/SCMT需求列表.xlsx
+++ b/Doc/需求分析/SCMT需求列表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="需求列表" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="功能列表——配置管理" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">需求列表!$A$1:$J$1</definedName>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="235">
   <si>
     <t>需求编号</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -858,12 +858,89 @@
     <t>用户组管理：按照用户组区分操作集</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>对象树</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCMT详细功能列表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能项</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>详细说明</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>主界面</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能点</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现日期</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建日期：2018-3-30
+更新日期：2018-3-30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、基站管理功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、GetResponse接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、GetNext接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、SetResponse接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>子项目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、SNMP模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、消息管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、MIB数据库JSON设计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -918,8 +995,52 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -938,8 +1059,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -997,11 +1123,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1076,15 +1259,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="标题 1" xfId="1" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="2" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="3" builtinId="18"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="4" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1133,7 +1376,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1166,9 +1409,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1201,6 +1461,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1379,19 +1656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="9" style="5"/>
-    <col min="4" max="4" width="35.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="62.375" style="8" customWidth="1"/>
     <col min="5" max="5" width="21.625" style="12" customWidth="1"/>
     <col min="9" max="9" width="22.25" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5">
+    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.15">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -1416,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1">
+    <row r="2" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1433,7 +1710,7 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
     </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1">
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="s">
         <v>72</v>
@@ -1450,7 +1727,7 @@
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:10" ht="27">
+    <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="16"/>
       <c r="B4" s="16" t="s">
         <v>16</v>
@@ -1471,7 +1748,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:10" ht="40.5">
+    <row r="5" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
       <c r="B5" s="10" t="s">
         <v>73</v>
@@ -1492,7 +1769,7 @@
       </c>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:10" ht="40.5">
+    <row r="6" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="16"/>
       <c r="B6" s="16" t="s">
         <v>74</v>
@@ -1511,7 +1788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="27">
+    <row r="7" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="B7" s="10" t="s">
         <v>75</v>
@@ -1528,7 +1805,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:10" ht="27">
+    <row r="8" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="17" t="s">
@@ -1548,7 +1825,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="27">
+    <row r="9" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="17" t="s">
@@ -1563,7 +1840,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:10" ht="54">
+    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.15">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="17" t="s">
@@ -1580,7 +1857,7 @@
       <c r="H10" s="21"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:10" ht="27">
+    <row r="11" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="17" t="s">
@@ -1597,7 +1874,7 @@
       <c r="H11" s="21"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:10" ht="27">
+    <row r="12" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="17" t="s">
@@ -1614,7 +1891,7 @@
       <c r="H12" s="21"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="17" t="s">
@@ -1629,7 +1906,7 @@
       <c r="H13" s="21"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:10" ht="27">
+    <row r="14" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="16"/>
       <c r="B14" s="16" t="s">
         <v>19</v>
@@ -1646,7 +1923,7 @@
       <c r="H14" s="21"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>203</v>
@@ -1663,7 +1940,7 @@
       <c r="H15" s="21"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="16"/>
       <c r="B16" s="16" t="s">
         <v>204</v>
@@ -1680,7 +1957,7 @@
       <c r="H16" s="21"/>
       <c r="I16" s="20"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>205</v>
@@ -1697,7 +1974,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="108">
+    <row r="18" spans="1:9" ht="108" x14ac:dyDescent="0.15">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>206</v>
@@ -1714,7 +1991,7 @@
       <c r="H18" s="21"/>
       <c r="I18" s="20"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="16"/>
       <c r="B19" s="16" t="s">
         <v>207</v>
@@ -1731,7 +2008,7 @@
       <c r="H19" s="21"/>
       <c r="I19" s="20"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="16"/>
       <c r="B20" s="16" t="s">
         <v>208</v>
@@ -1748,7 +2025,7 @@
       <c r="H20" s="21"/>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="27">
+    <row r="21" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>209</v>
@@ -1765,7 +2042,7 @@
       <c r="H21" s="21"/>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="24">
         <v>2</v>
       </c>
@@ -1784,7 +2061,7 @@
       <c r="H22" s="16"/>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" s="24"/>
       <c r="B23" s="16" t="s">
         <v>40</v>
@@ -1799,7 +2076,7 @@
       <c r="H23" s="16"/>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9" ht="81">
+    <row r="24" spans="1:9" ht="81" x14ac:dyDescent="0.15">
       <c r="A24" s="24"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16" t="s">
@@ -1816,7 +2093,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="25"/>
     </row>
-    <row r="25" spans="1:9" ht="27">
+    <row r="25" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A25" s="24"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16" t="s">
@@ -1833,7 +2110,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="1:9" ht="27">
+    <row r="26" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="24"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16" t="s">
@@ -1850,7 +2127,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="1:9" ht="27">
+    <row r="27" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A27" s="24"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16" t="s">
@@ -1867,7 +2144,7 @@
       <c r="H27" s="16"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" spans="1:9" ht="27">
+    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A28" s="24"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
@@ -1884,7 +2161,7 @@
       <c r="H28" s="16"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" spans="1:9" ht="27">
+    <row r="29" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="24"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16" t="s">
@@ -1901,7 +2178,7 @@
       <c r="H29" s="16"/>
       <c r="I29" s="25"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="24"/>
       <c r="B30" s="16" t="s">
         <v>47</v>
@@ -1918,7 +2195,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="25"/>
     </row>
-    <row r="31" spans="1:9" ht="40.5">
+    <row r="31" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A31" s="24"/>
       <c r="B31" s="16"/>
       <c r="C31" s="24" t="s">
@@ -1935,7 +2212,7 @@
       <c r="H31" s="16"/>
       <c r="I31" s="25"/>
     </row>
-    <row r="32" spans="1:9" ht="27">
+    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="24"/>
       <c r="B32" s="16"/>
       <c r="C32" s="24" t="s">
@@ -1952,7 +2229,7 @@
       <c r="H32" s="16"/>
       <c r="I32" s="25"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="24"/>
       <c r="B33" s="16"/>
       <c r="C33" s="24" t="s">
@@ -1969,7 +2246,7 @@
       <c r="H33" s="16"/>
       <c r="I33" s="25"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="24">
         <v>3</v>
       </c>
@@ -1986,7 +2263,7 @@
       <c r="H34" s="16"/>
       <c r="I34" s="25"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" s="24"/>
       <c r="B35" s="16" t="s">
         <v>51</v>
@@ -2003,7 +2280,7 @@
       <c r="H35" s="16"/>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" s="24"/>
       <c r="B36" s="16"/>
       <c r="C36" s="24" t="s">
@@ -2020,7 +2297,7 @@
       <c r="H36" s="16"/>
       <c r="I36" s="25"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="24"/>
       <c r="B37" s="16"/>
       <c r="C37" s="24" t="s">
@@ -2037,7 +2314,7 @@
       <c r="H37" s="16"/>
       <c r="I37" s="25"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="24"/>
       <c r="B38" s="16"/>
       <c r="C38" s="24" t="s">
@@ -2054,7 +2331,7 @@
       <c r="H38" s="16"/>
       <c r="I38" s="25"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="24"/>
       <c r="B39" s="16"/>
       <c r="C39" s="24" t="s">
@@ -2071,7 +2348,7 @@
       <c r="H39" s="16"/>
       <c r="I39" s="25"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="24"/>
       <c r="B40" s="16" t="s">
         <v>61</v>
@@ -2086,7 +2363,7 @@
       <c r="H40" s="16"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="24"/>
       <c r="B41" s="16"/>
       <c r="C41" s="24" t="s">
@@ -2103,7 +2380,7 @@
       <c r="H41" s="16"/>
       <c r="I41" s="25"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="24"/>
       <c r="B42" s="16"/>
       <c r="C42" s="24" t="s">
@@ -2120,7 +2397,7 @@
       <c r="H42" s="16"/>
       <c r="I42" s="25"/>
     </row>
-    <row r="43" spans="1:9" ht="27">
+    <row r="43" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="24"/>
       <c r="B43" s="16"/>
       <c r="C43" s="24" t="s">
@@ -2137,7 +2414,7 @@
       <c r="H43" s="16"/>
       <c r="I43" s="25"/>
     </row>
-    <row r="44" spans="1:9" ht="27">
+    <row r="44" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A44" s="24"/>
       <c r="B44" s="16"/>
       <c r="C44" s="24" t="s">
@@ -2154,7 +2431,7 @@
       <c r="H44" s="16"/>
       <c r="I44" s="25"/>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="24"/>
       <c r="B45" s="16"/>
       <c r="C45" s="24" t="s">
@@ -2171,7 +2448,7 @@
       <c r="H45" s="16"/>
       <c r="I45" s="25"/>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A46" s="24"/>
       <c r="B46" s="16"/>
       <c r="C46" s="24" t="s">
@@ -2188,7 +2465,7 @@
       <c r="H46" s="16"/>
       <c r="I46" s="25"/>
     </row>
-    <row r="47" spans="1:9" ht="27">
+    <row r="47" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A47" s="24"/>
       <c r="B47" s="16"/>
       <c r="C47" s="24" t="s">
@@ -2205,7 +2482,7 @@
       <c r="H47" s="16"/>
       <c r="I47" s="25"/>
     </row>
-    <row r="48" spans="1:9" ht="27">
+    <row r="48" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A48" s="24"/>
       <c r="B48" s="16"/>
       <c r="C48" s="24" t="s">
@@ -2222,7 +2499,7 @@
       <c r="H48" s="16"/>
       <c r="I48" s="25"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" s="24"/>
       <c r="B49" s="16"/>
       <c r="C49" s="24" t="s">
@@ -2239,7 +2516,7 @@
       <c r="H49" s="16"/>
       <c r="I49" s="25"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="24"/>
       <c r="B50" s="16"/>
       <c r="C50" s="24" t="s">
@@ -2256,7 +2533,7 @@
       <c r="H50" s="16"/>
       <c r="I50" s="25"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51" s="24"/>
       <c r="B51" s="16"/>
       <c r="C51" s="24" t="s">
@@ -2273,7 +2550,7 @@
       <c r="H51" s="16"/>
       <c r="I51" s="25"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A52" s="24">
         <v>4</v>
       </c>
@@ -2290,7 +2567,7 @@
       <c r="H52" s="16"/>
       <c r="I52" s="25"/>
     </row>
-    <row r="53" spans="1:9" ht="40.5">
+    <row r="53" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A53" s="24"/>
       <c r="B53" s="16" t="s">
         <v>82</v>
@@ -2307,7 +2584,7 @@
       <c r="H53" s="16"/>
       <c r="I53" s="25"/>
     </row>
-    <row r="54" spans="1:9" ht="40.5">
+    <row r="54" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A54" s="24">
         <v>5</v>
       </c>
@@ -2322,7 +2599,7 @@
       <c r="H54" s="16"/>
       <c r="I54" s="25"/>
     </row>
-    <row r="55" spans="1:9" ht="27">
+    <row r="55" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="24"/>
       <c r="B55" s="16" t="s">
         <v>146</v>
@@ -2339,7 +2616,7 @@
       <c r="H55" s="16"/>
       <c r="I55" s="25"/>
     </row>
-    <row r="56" spans="1:9" ht="40.5">
+    <row r="56" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A56" s="24"/>
       <c r="B56" s="16" t="s">
         <v>147</v>
@@ -2356,7 +2633,7 @@
       <c r="H56" s="16"/>
       <c r="I56" s="25"/>
     </row>
-    <row r="57" spans="1:9" ht="27">
+    <row r="57" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A57" s="24"/>
       <c r="B57" s="16" t="s">
         <v>150</v>
@@ -2373,7 +2650,7 @@
       <c r="H57" s="16"/>
       <c r="I57" s="25"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A58" s="24"/>
       <c r="B58" s="16"/>
       <c r="C58" s="24" t="s">
@@ -2390,7 +2667,7 @@
       <c r="H58" s="16"/>
       <c r="I58" s="25"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A59" s="24"/>
       <c r="B59" s="16"/>
       <c r="C59" s="24" t="s">
@@ -2407,7 +2684,7 @@
       <c r="H59" s="16"/>
       <c r="I59" s="25"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A60" s="24"/>
       <c r="B60" s="16"/>
       <c r="C60" s="24" t="s">
@@ -2424,7 +2701,7 @@
       <c r="H60" s="16"/>
       <c r="I60" s="25"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A61" s="24"/>
       <c r="B61" s="16"/>
       <c r="C61" s="24" t="s">
@@ -2441,7 +2718,7 @@
       <c r="H61" s="16"/>
       <c r="I61" s="25"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A62" s="24"/>
       <c r="B62" s="16"/>
       <c r="C62" s="24" t="s">
@@ -2458,7 +2735,7 @@
       <c r="H62" s="16"/>
       <c r="I62" s="25"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A63" s="24"/>
       <c r="B63" s="16"/>
       <c r="C63" s="24" t="s">
@@ -2475,7 +2752,7 @@
       <c r="H63" s="16"/>
       <c r="I63" s="25"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A64" s="24"/>
       <c r="B64" s="16"/>
       <c r="C64" s="24" t="s">
@@ -2492,7 +2769,7 @@
       <c r="H64" s="16"/>
       <c r="I64" s="25"/>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A65" s="24"/>
       <c r="B65" s="16"/>
       <c r="C65" s="24" t="s">
@@ -2509,7 +2786,7 @@
       <c r="H65" s="16"/>
       <c r="I65" s="25"/>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A66" s="24"/>
       <c r="B66" s="16" t="s">
         <v>151</v>
@@ -2526,7 +2803,7 @@
       <c r="H66" s="16"/>
       <c r="I66" s="25"/>
     </row>
-    <row r="67" spans="1:9" ht="27">
+    <row r="67" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A67" s="24"/>
       <c r="B67" s="16" t="s">
         <v>152</v>
@@ -2543,7 +2820,7 @@
       <c r="H67" s="16"/>
       <c r="I67" s="25"/>
     </row>
-    <row r="68" spans="1:9" ht="27">
+    <row r="68" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A68" s="24"/>
       <c r="B68" s="16" t="s">
         <v>153</v>
@@ -2560,7 +2837,7 @@
       <c r="H68" s="16"/>
       <c r="I68" s="25"/>
     </row>
-    <row r="69" spans="1:9" ht="27">
+    <row r="69" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A69" s="24"/>
       <c r="B69" s="16" t="s">
         <v>163</v>
@@ -2577,7 +2854,7 @@
       <c r="H69" s="16"/>
       <c r="I69" s="25"/>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A70" s="24"/>
       <c r="B70" s="16" t="s">
         <v>177</v>
@@ -2594,7 +2871,7 @@
       <c r="H70" s="16"/>
       <c r="I70" s="25"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A71" s="24"/>
       <c r="B71" s="16" t="s">
         <v>178</v>
@@ -2611,7 +2888,7 @@
       <c r="H71" s="16"/>
       <c r="I71" s="25"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A72" s="24">
         <v>6</v>
       </c>
@@ -2626,7 +2903,7 @@
       <c r="H72" s="16"/>
       <c r="I72" s="25"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A73" s="16"/>
       <c r="B73" s="16" t="s">
         <v>156</v>
@@ -2643,7 +2920,7 @@
       <c r="H73" s="16"/>
       <c r="I73" s="25"/>
     </row>
-    <row r="74" spans="1:9" ht="27">
+    <row r="74" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A74" s="16"/>
       <c r="B74" s="16" t="s">
         <v>158</v>
@@ -2660,7 +2937,7 @@
       <c r="H74" s="16"/>
       <c r="I74" s="25"/>
     </row>
-    <row r="75" spans="1:9" ht="27">
+    <row r="75" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A75" s="16"/>
       <c r="B75" s="16" t="s">
         <v>84</v>
@@ -2679,7 +2956,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A76" s="16"/>
       <c r="B76" s="16" t="s">
         <v>85</v>
@@ -2698,7 +2975,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A77" s="24">
         <v>7</v>
       </c>
@@ -2717,7 +2994,7 @@
       <c r="H77" s="16"/>
       <c r="I77" s="25"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A78" s="24"/>
       <c r="B78" s="16"/>
       <c r="C78" s="24" t="s">
@@ -2734,7 +3011,7 @@
       <c r="H78" s="16"/>
       <c r="I78" s="25"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A79" s="24"/>
       <c r="B79" s="16"/>
       <c r="C79" s="24" t="s">
@@ -2751,7 +3028,7 @@
       <c r="H79" s="16"/>
       <c r="I79" s="25"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A80" s="24">
         <v>8</v>
       </c>
@@ -2770,7 +3047,7 @@
       <c r="H80" s="16"/>
       <c r="I80" s="25"/>
     </row>
-    <row r="81" spans="1:9" ht="40.5">
+    <row r="81" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A81" s="24"/>
       <c r="B81" s="16" t="s">
         <v>111</v>
@@ -2787,7 +3064,7 @@
       <c r="H81" s="16"/>
       <c r="I81" s="25"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A82" s="16"/>
       <c r="B82" s="16" t="s">
         <v>112</v>
@@ -2804,7 +3081,7 @@
       <c r="H82" s="16"/>
       <c r="I82" s="25"/>
     </row>
-    <row r="83" spans="1:9" ht="27">
+    <row r="83" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A83" s="16"/>
       <c r="B83" s="16" t="s">
         <v>113</v>
@@ -2821,7 +3098,7 @@
       <c r="H83" s="16"/>
       <c r="I83" s="25"/>
     </row>
-    <row r="84" spans="1:9" ht="27">
+    <row r="84" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A84" s="16"/>
       <c r="B84" s="16" t="s">
         <v>114</v>
@@ -2838,7 +3115,7 @@
       <c r="H84" s="16"/>
       <c r="I84" s="25"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A85" s="24">
         <v>9</v>
       </c>
@@ -2857,7 +3134,7 @@
       <c r="H85" s="16"/>
       <c r="I85" s="25"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A86" s="24"/>
       <c r="B86" s="16" t="s">
         <v>110</v>
@@ -2874,7 +3151,7 @@
       <c r="H86" s="16"/>
       <c r="I86" s="25"/>
     </row>
-    <row r="87" spans="1:9" ht="27">
+    <row r="87" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A87" s="24"/>
       <c r="B87" s="16" t="s">
         <v>115</v>
@@ -2891,7 +3168,7 @@
       <c r="H87" s="16"/>
       <c r="I87" s="25"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A88" s="24">
         <v>10</v>
       </c>
@@ -2908,7 +3185,7 @@
       <c r="H88" s="16"/>
       <c r="I88" s="25"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A89" s="24">
         <v>11</v>
       </c>
@@ -2923,7 +3200,7 @@
       <c r="H89" s="16"/>
       <c r="I89" s="25"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="16"/>
       <c r="B90" s="16" t="s">
         <v>86</v>
@@ -2938,7 +3215,7 @@
       <c r="H90" s="16"/>
       <c r="I90" s="25"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A91" s="16"/>
       <c r="B91" s="16" t="s">
         <v>87</v>
@@ -2955,7 +3232,7 @@
       <c r="H91" s="16"/>
       <c r="I91" s="25"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A92" s="16"/>
       <c r="B92" s="16" t="s">
         <v>89</v>
@@ -2972,7 +3249,7 @@
       <c r="H92" s="16"/>
       <c r="I92" s="25"/>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A93" s="16"/>
       <c r="B93" s="16" t="s">
         <v>90</v>
@@ -2991,7 +3268,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A94" s="16"/>
       <c r="B94" s="16" t="s">
         <v>92</v>
@@ -3010,7 +3287,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A95" s="16"/>
       <c r="B95" s="16" t="s">
         <v>95</v>
@@ -3027,7 +3304,7 @@
       <c r="H95" s="16"/>
       <c r="I95" s="25"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A96" s="16"/>
       <c r="B96" s="16" t="s">
         <v>97</v>
@@ -3044,7 +3321,7 @@
       <c r="H96" s="16"/>
       <c r="I96" s="25"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A97" s="16"/>
       <c r="B97" s="16" t="s">
         <v>99</v>
@@ -3061,7 +3338,7 @@
       <c r="H97" s="16"/>
       <c r="I97" s="25"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A98" s="16"/>
       <c r="B98" s="16" t="s">
         <v>101</v>
@@ -3078,7 +3355,7 @@
       <c r="H98" s="16"/>
       <c r="I98" s="25"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A99" s="16"/>
       <c r="B99" s="16" t="s">
         <v>105</v>
@@ -3095,7 +3372,7 @@
       <c r="H99" s="16"/>
       <c r="I99" s="25"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A100" s="16"/>
       <c r="B100" s="16" t="s">
         <v>127</v>
@@ -3112,7 +3389,7 @@
       <c r="H100" s="16"/>
       <c r="I100" s="25"/>
     </row>
-    <row r="101" spans="1:9" ht="27">
+    <row r="101" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A101" s="24">
         <v>13</v>
       </c>
@@ -3129,7 +3406,7 @@
       <c r="H101" s="16"/>
       <c r="I101" s="25"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A102" s="16"/>
       <c r="B102" s="16" t="s">
         <v>138</v>
@@ -3146,7 +3423,7 @@
       <c r="H102" s="16"/>
       <c r="I102" s="25"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A103" s="16"/>
       <c r="B103" s="16" t="s">
         <v>139</v>
@@ -3163,7 +3440,7 @@
       <c r="H103" s="16"/>
       <c r="I103" s="25"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A104" s="16"/>
       <c r="B104" s="16" t="s">
         <v>140</v>
@@ -3180,7 +3457,7 @@
       <c r="H104" s="16"/>
       <c r="I104" s="25"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A105" s="16"/>
       <c r="B105" s="16" t="s">
         <v>141</v>
@@ -3197,7 +3474,7 @@
       <c r="H105" s="16"/>
       <c r="I105" s="25"/>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A106" s="16"/>
       <c r="B106" s="16"/>
       <c r="C106" s="24"/>
@@ -3208,7 +3485,7 @@
       <c r="H106" s="16"/>
       <c r="I106" s="25"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A107" s="16"/>
       <c r="B107" s="16"/>
       <c r="C107" s="24"/>
@@ -3219,7 +3496,7 @@
       <c r="H107" s="16"/>
       <c r="I107" s="25"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="4"/>
@@ -3230,7 +3507,7 @@
       <c r="H108" s="2"/>
       <c r="I108" s="11"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="4"/>
@@ -3241,7 +3518,7 @@
       <c r="H109" s="2"/>
       <c r="I109" s="11"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="4"/>
@@ -3252,7 +3529,7 @@
       <c r="H110" s="2"/>
       <c r="I110" s="11"/>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="4"/>
@@ -3263,7 +3540,7 @@
       <c r="H111" s="2"/>
       <c r="I111" s="11"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="4"/>
@@ -3274,7 +3551,7 @@
       <c r="H112" s="2"/>
       <c r="I112" s="11"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="4"/>
@@ -3285,7 +3562,7 @@
       <c r="H113" s="2"/>
       <c r="I113" s="11"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="4"/>
@@ -3296,7 +3573,7 @@
       <c r="H114" s="2"/>
       <c r="I114" s="11"/>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="4"/>
@@ -3307,7 +3584,7 @@
       <c r="H115" s="2"/>
       <c r="I115" s="11"/>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="4"/>
@@ -3318,7 +3595,7 @@
       <c r="H116" s="2"/>
       <c r="I116" s="11"/>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="4"/>
@@ -3329,7 +3606,7 @@
       <c r="H117" s="2"/>
       <c r="I117" s="11"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="4"/>
@@ -3340,7 +3617,7 @@
       <c r="H118" s="2"/>
       <c r="I118" s="11"/>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="4"/>
@@ -3351,7 +3628,7 @@
       <c r="H119" s="2"/>
       <c r="I119" s="11"/>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="4"/>
@@ -3362,7 +3639,7 @@
       <c r="H120" s="2"/>
       <c r="I120" s="11"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="4"/>
@@ -3373,7 +3650,7 @@
       <c r="H121" s="2"/>
       <c r="I121" s="11"/>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="4"/>
@@ -3384,7 +3661,7 @@
       <c r="H122" s="2"/>
       <c r="I122" s="11"/>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="4"/>
@@ -3395,7 +3672,7 @@
       <c r="H123" s="2"/>
       <c r="I123" s="11"/>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="4"/>
@@ -3406,7 +3683,7 @@
       <c r="H124" s="2"/>
       <c r="I124" s="11"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="4"/>
@@ -3417,7 +3694,7 @@
       <c r="H125" s="2"/>
       <c r="I125" s="11"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="4"/>
@@ -3428,7 +3705,7 @@
       <c r="H126" s="2"/>
       <c r="I126" s="11"/>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="4"/>
@@ -3439,7 +3716,7 @@
       <c r="H127" s="2"/>
       <c r="I127" s="11"/>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C128" s="9"/>
       <c r="D128" s="7"/>
       <c r="E128" s="11"/>
@@ -3469,13 +3746,222 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="5" customWidth="1"/>
+    <col min="3" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="27.25" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="6.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="46"/>
+      <c r="B7" s="44"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="46"/>
+      <c r="B8" s="44"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="46"/>
+      <c r="B9" s="44"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="46"/>
+      <c r="B10" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="37">
+        <v>43110</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="46"/>
+      <c r="B11" s="44"/>
+      <c r="C11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="37">
+        <v>43110</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="46"/>
+      <c r="B12" s="44"/>
+      <c r="C12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F12" s="37">
+        <v>43110</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="46"/>
+      <c r="B13" s="45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="46"/>
+      <c r="B14" s="45"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="46"/>
+      <c r="B15" s="45"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="47"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="48"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="48"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="48"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="48"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="48"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="48" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="39"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="39"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="39"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="39"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" s="39"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="39"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C5:E5"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update No Title problem
</commit_message>
<xml_diff>
--- a/Doc/需求分析/SCMT需求列表.xlsx
+++ b/Doc/需求分析/SCMT需求列表.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EA53AAE3-13AA-4951-84A8-A315084A07CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="需求列表" sheetId="1" r:id="rId1"/>
-    <sheet name="功能列表——配置管理" sheetId="3" r:id="rId2"/>
+    <sheet name="细化需求列表——配置管理" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">需求列表!$A$1:$J$1</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="262">
   <si>
     <t>需求编号</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -875,10 +876,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>主界面</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>功能点</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -896,10 +893,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>1、基站管理功能</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>核心功能</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -932,14 +925,130 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>3、MIB数据库JSON设计</t>
+    <t>UI布局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、图表显示功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、DataGrid图表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、折线图表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、3D折线图表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现方案</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、对象树显示</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、配置管理功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、“日历”图</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CefSharp+Echart方案</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注与补充</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>封装SNMPSharpNet</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用NewtonSoft.Json实现</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、对象树JSON解析与显示</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、MIB表JSON解析与查询接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、SI模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5、MIB数据库JSON设计</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、FTP模块</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、TCP链路</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>.NET默认TcpClient</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、基站建链接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、UE信息查询接口</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4、多基站管理</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、用户交互功能</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、界面元素拖拽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2、拖拽后释放事件触发</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3、用户界面自由布局</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avalon</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1160,11 +1269,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1184,7 +1295,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1253,27 +1364,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1281,35 +1391,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1653,11 +1777,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1669,11 +1793,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1748,7 +1872,7 @@
       </c>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
       <c r="B5" s="10" t="s">
         <v>73</v>
@@ -1788,7 +1912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="16"/>
       <c r="B7" s="10" t="s">
         <v>75</v>
@@ -1805,7 +1929,7 @@
       <c r="H7" s="21"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="17" t="s">
@@ -1840,7 +1964,7 @@
       <c r="H9" s="21"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:10" ht="54" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="17" t="s">
@@ -1974,7 +2098,7 @@
       <c r="H17" s="21"/>
       <c r="I17" s="20"/>
     </row>
-    <row r="18" spans="1:9" ht="108" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>206</v>
@@ -2025,7 +2149,7 @@
       <c r="H20" s="21"/>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>209</v>
@@ -2076,7 +2200,7 @@
       <c r="H23" s="16"/>
       <c r="I23" s="25"/>
     </row>
-    <row r="24" spans="1:9" ht="81" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A24" s="24"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16" t="s">
@@ -2093,7 +2217,7 @@
       <c r="H24" s="16"/>
       <c r="I24" s="25"/>
     </row>
-    <row r="25" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="24"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16" t="s">
@@ -2110,7 +2234,7 @@
       <c r="H25" s="16"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="24"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16" t="s">
@@ -2127,7 +2251,7 @@
       <c r="H26" s="16"/>
       <c r="I26" s="25"/>
     </row>
-    <row r="27" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="24"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16" t="s">
@@ -2144,7 +2268,7 @@
       <c r="H27" s="16"/>
       <c r="I27" s="25"/>
     </row>
-    <row r="28" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="24"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16" t="s">
@@ -2161,7 +2285,7 @@
       <c r="H28" s="16"/>
       <c r="I28" s="25"/>
     </row>
-    <row r="29" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="24"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16" t="s">
@@ -2195,7 +2319,7 @@
       <c r="H30" s="16"/>
       <c r="I30" s="25"/>
     </row>
-    <row r="31" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="24"/>
       <c r="B31" s="16"/>
       <c r="C31" s="24" t="s">
@@ -2212,7 +2336,7 @@
       <c r="H31" s="16"/>
       <c r="I31" s="25"/>
     </row>
-    <row r="32" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="24"/>
       <c r="B32" s="16"/>
       <c r="C32" s="24" t="s">
@@ -2397,7 +2521,7 @@
       <c r="H42" s="16"/>
       <c r="I42" s="25"/>
     </row>
-    <row r="43" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="24"/>
       <c r="B43" s="16"/>
       <c r="C43" s="24" t="s">
@@ -2414,7 +2538,7 @@
       <c r="H43" s="16"/>
       <c r="I43" s="25"/>
     </row>
-    <row r="44" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="24"/>
       <c r="B44" s="16"/>
       <c r="C44" s="24" t="s">
@@ -2465,7 +2589,7 @@
       <c r="H46" s="16"/>
       <c r="I46" s="25"/>
     </row>
-    <row r="47" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A47" s="24"/>
       <c r="B47" s="16"/>
       <c r="C47" s="24" t="s">
@@ -2482,7 +2606,7 @@
       <c r="H47" s="16"/>
       <c r="I47" s="25"/>
     </row>
-    <row r="48" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A48" s="24"/>
       <c r="B48" s="16"/>
       <c r="C48" s="24" t="s">
@@ -2567,7 +2691,7 @@
       <c r="H52" s="16"/>
       <c r="I52" s="25"/>
     </row>
-    <row r="53" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A53" s="24"/>
       <c r="B53" s="16" t="s">
         <v>82</v>
@@ -2584,7 +2708,7 @@
       <c r="H53" s="16"/>
       <c r="I53" s="25"/>
     </row>
-    <row r="54" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A54" s="24">
         <v>5</v>
       </c>
@@ -2599,7 +2723,7 @@
       <c r="H54" s="16"/>
       <c r="I54" s="25"/>
     </row>
-    <row r="55" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A55" s="24"/>
       <c r="B55" s="16" t="s">
         <v>146</v>
@@ -2616,7 +2740,7 @@
       <c r="H55" s="16"/>
       <c r="I55" s="25"/>
     </row>
-    <row r="56" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A56" s="24"/>
       <c r="B56" s="16" t="s">
         <v>147</v>
@@ -2820,7 +2944,7 @@
       <c r="H67" s="16"/>
       <c r="I67" s="25"/>
     </row>
-    <row r="68" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A68" s="24"/>
       <c r="B68" s="16" t="s">
         <v>153</v>
@@ -2837,7 +2961,7 @@
       <c r="H68" s="16"/>
       <c r="I68" s="25"/>
     </row>
-    <row r="69" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" s="24"/>
       <c r="B69" s="16" t="s">
         <v>163</v>
@@ -2920,7 +3044,7 @@
       <c r="H73" s="16"/>
       <c r="I73" s="25"/>
     </row>
-    <row r="74" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A74" s="16"/>
       <c r="B74" s="16" t="s">
         <v>158</v>
@@ -2937,7 +3061,7 @@
       <c r="H74" s="16"/>
       <c r="I74" s="25"/>
     </row>
-    <row r="75" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A75" s="16"/>
       <c r="B75" s="16" t="s">
         <v>84</v>
@@ -3047,7 +3171,7 @@
       <c r="H80" s="16"/>
       <c r="I80" s="25"/>
     </row>
-    <row r="81" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:9" ht="27" x14ac:dyDescent="0.15">
       <c r="A81" s="24"/>
       <c r="B81" s="16" t="s">
         <v>111</v>
@@ -3151,7 +3275,7 @@
       <c r="H86" s="16"/>
       <c r="I86" s="25"/>
     </row>
-    <row r="87" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A87" s="24"/>
       <c r="B87" s="16" t="s">
         <v>115</v>
@@ -3389,7 +3513,7 @@
       <c r="H100" s="16"/>
       <c r="I100" s="25"/>
     </row>
-    <row r="101" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A101" s="24">
         <v>13</v>
       </c>
@@ -3726,7 +3850,7 @@
       <c r="I128" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1">
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0" showButton="0"/>
     <filterColumn colId="1" showButton="0"/>
   </autoFilter>
@@ -3735,7 +3859,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3745,11 +3869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3759,43 +3883,43 @@
     <col min="3" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="27.25" customWidth="1"/>
     <col min="5" max="5" width="28.5" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="37" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="29" customWidth="1"/>
     <col min="7" max="7" width="6.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="38" t="s">
-        <v>223</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="A2" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="27" t="s">
         <v>218</v>
       </c>
       <c r="B4" s="33" t="s">
@@ -3804,161 +3928,715 @@
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
-      <c r="F4" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="G4" s="30" t="s">
+      <c r="F4" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="51" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>231</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="46" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="52"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="52"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="52"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="52"/>
+      <c r="B10" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="43">
+        <v>43110</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="52"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="D11" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="43">
+        <v>43110</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="52"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="43">
+        <v>43110</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="52"/>
+      <c r="B13" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="52"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="52"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="52"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="52"/>
+      <c r="B17" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="52"/>
+      <c r="B18" s="46" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="52"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="52"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="52"/>
+      <c r="B21" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="53"/>
+      <c r="B22" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="47"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="41" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="41"/>
+      <c r="B25" s="42" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="46"/>
-      <c r="B7" s="44"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="46"/>
-      <c r="B8" s="44"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="46"/>
-      <c r="B9" s="44"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="46"/>
-      <c r="B10" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C10" t="s">
-        <v>227</v>
-      </c>
-      <c r="F10" s="37">
-        <v>43110</v>
-      </c>
-      <c r="G10" s="40" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="46"/>
-      <c r="B11" s="44"/>
-      <c r="C11" t="s">
-        <v>228</v>
-      </c>
-      <c r="F11" s="37">
-        <v>43110</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="46"/>
-      <c r="B12" s="44"/>
-      <c r="C12" t="s">
-        <v>229</v>
-      </c>
-      <c r="F12" s="37">
-        <v>43110</v>
-      </c>
-      <c r="G12" s="40" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="46"/>
-      <c r="B13" s="45" t="s">
+      <c r="C25" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="46"/>
-      <c r="B14" s="45"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="46"/>
-      <c r="B15" s="45"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="47"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="48" t="s">
-        <v>220</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="48"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="48"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="48"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="48"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="48"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="48" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="41"/>
+      <c r="B29" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="41"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="41"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="49"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="49" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="39"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="39"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="39"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="39"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="39"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="39"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="39"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="50"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="50"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="50"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="50"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="50"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="50"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="50"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="2"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="2"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="43"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="2"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="2"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A45" s="2"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="43"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A46" s="2"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="43"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="2"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A48" s="2"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A49" s="2"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="43"/>
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A50" s="2"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="43"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A51" s="2"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A52" s="2"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="43"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A53" s="2"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A54" s="2"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="43"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A55" s="2"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="43"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A56" s="2"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="43"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A57" s="2"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="43"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A58" s="2"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="43"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A59" s="2"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="43"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A60" s="2"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A61" s="2"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A62" s="2"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="43"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A63" s="2"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="43"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A64" s="2"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="43"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A65" s="2"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="2"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A66" s="2"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="43"/>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A67" s="2"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A68" s="2"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="43"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A69" s="2"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="2"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A70" s="2"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="43"/>
+      <c r="G70" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A6:A22"/>
     <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="B18:B20"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="A2:D3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>